<commit_message>
Made creation of DB/Tables if not exists, fleshed out new term/upload data page of test.html
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="185">
   <si>
     <t>Item</t>
   </si>
@@ -549,15 +549,6 @@
     <t>Table</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
     <t>Table Size</t>
   </si>
   <si>
@@ -577,6 +568,15 @@
   </si>
   <si>
     <t>Position Type</t>
+  </si>
+  <si>
+    <t>Rich-Husbands-In-Training (RHIT)</t>
+  </si>
+  <si>
+    <t>Electrical Engineering, Computer Science</t>
+  </si>
+  <si>
+    <t>US Citizen,H-1 Visa</t>
   </si>
 </sst>
 </file>
@@ -894,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,57 +912,41 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>2015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" t="s">
-        <v>177</v>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
         <v>10</v>
       </c>
     </row>
@@ -975,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -994,7 +978,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1002,7 +986,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1010,7 +994,7 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1018,7 +1002,7 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1026,7 +1010,7 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1034,7 +1018,7 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1042,7 +1026,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1050,7 +1034,7 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1058,7 +1042,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1066,7 +1050,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1074,7 +1058,7 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1082,7 +1066,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1090,7 +1074,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1098,7 +1082,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1106,7 +1090,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1114,7 +1098,7 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1122,7 +1106,7 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1130,7 +1114,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,7 +1122,7 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1146,7 +1130,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1154,7 +1138,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,7 +1146,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1170,7 +1154,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1178,7 +1162,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1186,7 +1170,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,7 +1178,7 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1202,7 +1186,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1194,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1226,7 +1210,7 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1234,7 +1218,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1242,7 +1226,7 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1250,7 +1234,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1258,7 +1242,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1266,7 +1250,7 @@
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1274,7 +1258,7 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1284,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,13 +1285,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -2117,180 +2101,180 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>182</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="E49">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="D50" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E50">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E51">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C52" t="s">
         <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E52">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D53" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E53">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C54" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="D54" t="s">
         <v>51</v>
       </c>
       <c r="E54">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E55">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E56">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="D57" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="E57">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E58">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
@@ -2299,100 +2283,100 @@
         <v>12</v>
       </c>
       <c r="E59">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E60">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E61">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E62">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
         <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E63">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C64" t="s">
         <v>17</v>
       </c>
       <c r="D64" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E64">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
@@ -2401,108 +2385,125 @@
         <v>51</v>
       </c>
       <c r="E65">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E66">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E67">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C68" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E68">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
       </c>
       <c r="E69">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>50</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>49</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>48</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>47</v>
       </c>
-      <c r="E71">
+      <c r="E72">
         <v>13</v>
       </c>
     </row>
@@ -2523,13 +2524,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Allow undefined mappings to gracefully continue
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -897,7 +897,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +947,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic to handle cases where height is not provided
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -947,7 +947,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1270,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modified TermVars table to also have 'type' attribute
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="186">
   <si>
     <t>Item</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>US Citizen,H-1 Visa</t>
+  </si>
+  <si>
+    <t>Layout</t>
   </si>
 </sst>
 </file>
@@ -894,60 +897,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated logic to create terms
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="184">
   <si>
     <t>Item</t>
   </si>
@@ -169,12 +169,6 @@
   </si>
   <si>
     <t>US Citizen, Permanent Resident</t>
-  </si>
-  <si>
-    <t>Civil Engineering, Mechanical Engineering, Software Engineering</t>
-  </si>
-  <si>
-    <t>Wynright</t>
   </si>
   <si>
     <t>Internship/Externship, Full Time</t>
@@ -899,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -935,7 +929,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,7 +940,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,7 +951,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -968,7 +962,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +993,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1007,7 +1001,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1015,7 +1009,7 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1023,7 +1017,7 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1031,7 +1025,7 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1039,7 +1033,7 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,7 +1041,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,7 +1049,7 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1063,7 +1057,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1071,7 +1065,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1079,7 +1073,7 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1087,7 +1081,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1095,7 +1089,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1103,7 +1097,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,7 +1105,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1119,7 +1113,7 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1127,7 +1121,7 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1135,7 +1129,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,7 +1145,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1153,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1167,7 +1161,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1175,7 +1169,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,7 +1177,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1191,7 +1185,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1199,7 +1193,7 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,7 +1201,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1215,7 +1209,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1223,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1225,7 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1239,7 +1233,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1247,7 +1241,7 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1255,7 +1249,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1263,7 +1257,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1271,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1279,7 +1273,7 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1289,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,33 +1300,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1340,10 +1334,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1357,10 +1351,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -1374,16 +1368,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -1391,10 +1385,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1408,16 +1402,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E7">
         <v>48</v>
@@ -1425,7 +1419,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -1442,10 +1436,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
@@ -1459,7 +1453,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -1476,16 +1470,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11">
         <v>61</v>
@@ -1493,7 +1487,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -1502,7 +1496,7 @@
         <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12">
         <v>62</v>
@@ -1510,7 +1504,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1519,7 +1513,7 @@
         <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13">
         <v>38</v>
@@ -1527,16 +1521,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E14">
         <v>47</v>
@@ -1544,13 +1538,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -1561,16 +1555,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16">
         <v>49</v>
@@ -1578,10 +1572,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s">
         <v>48</v>
@@ -1595,16 +1589,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E18">
         <v>54</v>
@@ -1612,10 +1606,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1629,13 +1623,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1646,10 +1640,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -1663,10 +1657,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" t="s">
         <v>48</v>
@@ -1680,16 +1674,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -1697,16 +1691,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E24">
         <v>12</v>
@@ -1714,7 +1708,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -1723,7 +1717,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E25">
         <v>36</v>
@@ -1731,16 +1725,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E26">
         <v>31</v>
@@ -1748,7 +1742,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
@@ -1757,7 +1751,7 @@
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E27">
         <v>19</v>
@@ -1765,16 +1759,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E28">
         <v>44</v>
@@ -1782,16 +1776,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E29">
         <v>33</v>
@@ -1799,16 +1793,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C30" t="s">
         <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E30">
         <v>18</v>
@@ -1816,10 +1810,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
         <v>48</v>
@@ -1833,7 +1827,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -1850,16 +1844,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E33">
         <v>6</v>
@@ -1867,16 +1861,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
         <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E34">
         <v>21</v>
@@ -1884,13 +1878,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -1901,10 +1895,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
         <v>48</v>
@@ -1918,16 +1912,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1935,16 +1929,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E38">
         <v>43</v>
@@ -1952,16 +1946,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E39">
         <v>34</v>
@@ -1969,7 +1963,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
@@ -1978,7 +1972,7 @@
         <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E40">
         <v>25</v>
@@ -1986,16 +1980,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
         <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E41">
         <v>69</v>
@@ -2003,16 +1997,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E42">
         <v>63</v>
@@ -2020,13 +2014,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -2037,10 +2031,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
         <v>48</v>
@@ -2054,10 +2048,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
         <v>48</v>
@@ -2071,10 +2065,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -2088,16 +2082,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E47">
         <v>27</v>
@@ -2105,13 +2099,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -2122,16 +2116,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
         <v>182</v>
       </c>
-      <c r="B49" t="s">
-        <v>183</v>
-      </c>
-      <c r="C49" t="s">
-        <v>184</v>
-      </c>
       <c r="D49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E49">
         <v>56</v>
@@ -2139,13 +2133,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D50" t="s">
         <v>47</v>
@@ -2156,16 +2150,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E51">
         <v>42</v>
@@ -2173,7 +2167,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
         <v>38</v>
@@ -2190,10 +2184,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
         <v>48</v>
@@ -2207,16 +2201,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E54">
         <v>71</v>
@@ -2224,16 +2218,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E55">
         <v>60</v>
@@ -2241,10 +2235,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
@@ -2258,16 +2252,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E57">
         <v>10</v>
@@ -2275,16 +2269,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" t="s">
         <v>48</v>
       </c>
       <c r="D58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E58">
         <v>50</v>
@@ -2292,7 +2286,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B59" t="s">
         <v>23</v>
@@ -2309,10 +2303,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
@@ -2326,13 +2320,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D61" t="s">
         <v>47</v>
@@ -2343,7 +2337,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B62" t="s">
         <v>36</v>
@@ -2360,10 +2354,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
         <v>17</v>
@@ -2377,10 +2371,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C64" t="s">
         <v>17</v>
@@ -2394,16 +2388,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E65">
         <v>37</v>
@@ -2411,16 +2405,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E66">
         <v>14</v>
@@ -2428,7 +2422,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B67" t="s">
         <v>23</v>
@@ -2445,16 +2439,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
       </c>
       <c r="D68" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E68">
         <v>53</v>
@@ -2462,10 +2456,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
         <v>48</v>
@@ -2479,10 +2473,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
@@ -2496,36 +2490,19 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
         <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E71">
         <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>50</v>
-      </c>
-      <c r="B72" t="s">
-        <v>49</v>
-      </c>
-      <c r="C72" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" t="s">
-        <v>47</v>
-      </c>
-      <c r="E72">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2545,13 +2522,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed table generation procedures
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
@@ -2514,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>18</v>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>19</v>
@@ -2918,7 +2918,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>20</v>
@@ -2929,7 +2929,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>21</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>22</v>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>23</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>24</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>25</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>26</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>27</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>28</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>29</v>
@@ -3028,7 +3028,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>30</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>16</v>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49">
         <v>15</v>
@@ -3061,7 +3061,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>14</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <v>13</v>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52">
         <v>12</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>11</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>10</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55">
         <v>9</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56">
         <v>8</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57">
         <v>7</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58">
         <v>6</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -3182,7 +3182,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61">
         <v>3</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -3215,7 +3215,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B64">
         <v>63</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B65">
         <v>64</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B66">
         <v>65</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67">
         <v>66</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B68">
         <v>67</v>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B69">
         <v>68</v>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70">
         <v>69</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71">
         <v>70</v>
@@ -3303,7 +3303,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B72">
         <v>71</v>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B73">
         <v>72</v>

</xml_diff>

<commit_message>
Added checks to alert user that table may be in walkway
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>183</v>
@@ -2514,7 +2514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Make row single block if no walkway
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -894,7 +894,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>183</v>

</xml_diff>

<commit_message>
Prevent tables in different sections from being joined
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -894,7 +894,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>183</v>

</xml_diff>

<commit_message>
Changed to move tableNumbers into tableMapping
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="182">
   <si>
     <t>Item</t>
   </si>
@@ -540,16 +540,10 @@
     <t>Addenda/PAG Holdings</t>
   </si>
   <si>
-    <t>Table</t>
-  </si>
-  <si>
     <t>Table Size</t>
   </si>
   <si>
     <t>Table Number</t>
-  </si>
-  <si>
-    <t>Location</t>
   </si>
   <si>
     <t>Work Authorization</t>
@@ -893,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -918,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -929,7 +923,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -951,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -993,7 +987,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1001,7 +995,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1009,7 +1003,7 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1017,7 +1011,7 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1025,7 +1019,7 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1033,7 +1027,7 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1041,7 +1035,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1049,7 +1043,7 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1051,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1065,7 +1059,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1073,7 +1067,7 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1081,7 +1075,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1083,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1097,7 +1091,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1105,7 +1099,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1113,7 +1107,7 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1121,7 +1115,7 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1129,7 +1123,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1137,7 +1131,7 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1145,7 +1139,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1153,7 +1147,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1161,7 +1155,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1169,7 +1163,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1177,7 +1171,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1185,7 +1179,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1193,7 +1187,7 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1195,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1209,7 +1203,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1217,7 +1211,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1225,7 +1219,7 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1233,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1241,7 +1235,7 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1243,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,7 +1251,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1259,7 @@
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1273,7 +1267,7 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1285,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,19 +1294,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2116,13 +2110,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
         <v>180</v>
-      </c>
-      <c r="B49" t="s">
-        <v>181</v>
-      </c>
-      <c r="C49" t="s">
-        <v>182</v>
       </c>
       <c r="D49" t="s">
         <v>107</v>
@@ -2512,814 +2506,593 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>47</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>48</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>49</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>51</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>52</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>53</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>54</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>55</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>56</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>57</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>58</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>59</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>60</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>61</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>62</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>46</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>45</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>44</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>43</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>42</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>41</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>40</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>39</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>38</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>37</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>36</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>35</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>34</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>33</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>32</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>31</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>17</v>
-      </c>
-      <c r="C34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>18</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>19</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>20</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>21</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <v>22</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>23</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>24</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
-        <v>25</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
-        <v>26</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
-        <v>27</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
-        <v>28</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
-        <v>29</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
-        <v>30</v>
-      </c>
-      <c r="C47">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
-        <v>16</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
-        <v>15</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
-        <v>14</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
-        <v>13</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
-        <v>12</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
-        <v>11</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
-        <v>10</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
-        <v>9</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
-        <v>8</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
-        <v>7</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
-        <v>6</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
-        <v>5</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
-        <v>3</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
-        <v>2</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
-        <v>63</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
-        <v>64</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
-        <v>65</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
-        <v>66</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
-        <v>67</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
-        <v>68</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
-        <v>69</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
-        <v>70</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
-        <v>71</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
-        <v>72</v>
-      </c>
-      <c r="C73">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revised frontend to use new tableMapping and NWayMaps
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benedict\Documents\Work\Workspaces\OpenShift\rhcareerfairlayout\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\Workspaces\OpenShift\rhcareerfairlayout\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>181</v>
@@ -2506,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3098,6 +3098,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added tags, click-to assign, highlight companies in red if unassigned
</commit_message>
<xml_diff>
--- a/src/main/resources/Spring2015.xlsx
+++ b/src/main/resources/Spring2015.xlsx
@@ -2506,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:XFD76"/>
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3098,22 +3098,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>